<commit_message>
Simhash now works (the sketching part)
</commit_message>
<xml_diff>
--- a/Untitled-1.xlsx
+++ b/Untitled-1.xlsx
@@ -1,21 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ITU\kand\4.Semester\LSHonGPU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\petur\source\repos\ThesisParser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{AC5F4D10-97A3-454A-B589-854DC9823C38}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5CED27-5069-418F-8CAD-9E32109FD232}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Untitled-1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -52,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -886,524 +894,756 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AX19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:Z1"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1">
-        <v>0.27309</v>
+        <v>9.2177100000000003</v>
       </c>
       <c r="C1">
-        <v>0.60972000000000004</v>
+        <v>4.2579900000000004</v>
       </c>
       <c r="D1">
-        <v>-0.50971999999999995</v>
+        <v>4.4252200000000004</v>
       </c>
       <c r="E1">
-        <v>0.15690999999999999</v>
+        <v>0.397115</v>
       </c>
       <c r="F1">
-        <v>-0.32430999999999999</v>
+        <v>2.8813</v>
       </c>
       <c r="G1">
-        <v>0.16807</v>
+        <v>4.8769499999999999</v>
       </c>
       <c r="H1">
-        <v>1.7350000000000001</v>
+        <v>7.91005</v>
       </c>
       <c r="I1">
-        <v>-2.6096000000000001E-2</v>
+        <v>7.7086499999999996</v>
       </c>
       <c r="J1">
-        <v>0.1123</v>
+        <v>6.8506600000000004</v>
       </c>
       <c r="K1">
-        <v>0.19067000000000001</v>
+        <v>4.5134499999999997</v>
       </c>
       <c r="L1">
-        <v>4.0482999999999998E-2</v>
+        <v>8.0312199999999994</v>
       </c>
       <c r="M1">
-        <v>0.27916999999999997</v>
+        <v>5.39499</v>
       </c>
       <c r="N1">
-        <v>-4.992</v>
+        <v>7.0177300000000002</v>
       </c>
       <c r="O1">
-        <v>-0.69633999999999996</v>
+        <v>5.8789999999999996</v>
       </c>
       <c r="P1">
-        <v>-0.80095000000000005</v>
+        <v>5.8778899999999998</v>
       </c>
       <c r="Q1">
-        <v>0.38192999999999999</v>
+        <v>6.2914899999999996</v>
       </c>
       <c r="R1">
-        <v>0.47417999999999999</v>
+        <v>4.7436999999999996</v>
       </c>
       <c r="S1">
-        <v>-1.4587000000000001</v>
+        <v>1.6280300000000001</v>
       </c>
       <c r="T1">
-        <v>0.10963000000000001</v>
+        <v>8.5528600000000008</v>
       </c>
       <c r="U1">
-        <v>-0.75060000000000004</v>
+        <v>3.7722899999999999</v>
       </c>
       <c r="V1">
-        <v>-0.56681999999999999</v>
+        <v>5.9397200000000003</v>
       </c>
       <c r="W1">
-        <v>0.64329000000000003</v>
+        <v>3.8351999999999999</v>
       </c>
       <c r="X1">
-        <v>-0.18412999999999999</v>
+        <v>6.3369900000000001</v>
       </c>
       <c r="Y1">
-        <v>0.62394000000000005</v>
+        <v>4.7926099999999998</v>
       </c>
       <c r="Z1">
-        <v>-0.28699999999999998</v>
+        <v>5.2987700000000002</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0.62414999999999998</v>
+        <v>-0.47033000000000003</v>
       </c>
       <c r="C2">
-        <v>0.62475999999999998</v>
+        <v>-0.23693</v>
       </c>
       <c r="D2">
-        <v>-8.2335000000000005E-2</v>
+        <v>-1.4953000000000001</v>
       </c>
       <c r="E2">
-        <v>0.20100999999999999</v>
+        <v>-0.22986000000000001</v>
       </c>
       <c r="F2">
-        <v>-0.13741</v>
+        <v>-0.42457</v>
       </c>
       <c r="G2">
-        <v>-0.11430999999999999</v>
+        <v>-1.5589999999999999</v>
       </c>
       <c r="H2">
-        <v>0.77908999999999995</v>
+        <v>0.15847</v>
       </c>
       <c r="I2">
-        <v>2.6356000000000002</v>
+        <v>0.52688000000000001</v>
       </c>
       <c r="J2">
-        <v>-0.46350999999999998</v>
+        <v>-6.5265999999999996E-3</v>
       </c>
       <c r="K2">
-        <v>0.57464999999999999</v>
+        <v>1.0267999999999999</v>
       </c>
       <c r="L2">
-        <v>-2.4888E-2</v>
+        <v>0.16051000000000001</v>
       </c>
       <c r="M2">
-        <v>-1.5466000000000001E-2</v>
+        <v>-2.3574000000000002</v>
       </c>
       <c r="N2">
-        <v>-2.9695999999999998</v>
+        <v>-2.6055999999999999</v>
       </c>
       <c r="O2">
-        <v>-0.49875999999999998</v>
+        <v>3.3404000000000003E-2</v>
       </c>
       <c r="P2">
-        <v>9.5033999999999993E-2</v>
+        <v>-0.58252999999999999</v>
       </c>
       <c r="Q2">
-        <v>-0.94879000000000002</v>
+        <v>1.7386999999999999</v>
       </c>
       <c r="R2">
-        <v>-1.7336000000000001E-2</v>
+        <v>-0.98226999999999998</v>
       </c>
       <c r="S2">
-        <v>-0.86348999999999998</v>
+        <v>0.94823000000000002</v>
       </c>
       <c r="T2">
-        <v>-1.3348</v>
+        <v>-2.6023999999999998</v>
       </c>
       <c r="U2">
-        <v>4.6810999999999998E-2</v>
+        <v>-0.14505000000000001</v>
       </c>
       <c r="V2">
-        <v>0.36998999999999999</v>
+        <v>0.36788999999999999</v>
       </c>
       <c r="W2">
-        <v>-0.57662999999999998</v>
+        <v>0.32945000000000002</v>
       </c>
       <c r="X2">
-        <v>-0.48469000000000001</v>
+        <v>0.30675000000000002</v>
       </c>
       <c r="Y2">
-        <v>0.40078000000000003</v>
+        <v>-8.0438999999999997E-3</v>
       </c>
       <c r="Z2">
-        <v>0.75344999999999995</v>
+        <v>-0.41343999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
         <f>B1*B2</f>
-        <v>0.17044912349999999</v>
+        <v>-4.3353655443000001</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:Z3" si="0">C1*C2</f>
-        <v>0.38092866720000002</v>
+        <v>-1.0088455707000001</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>4.1967796199999997E-2</v>
+        <v>-6.6170314660000011</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>3.1540479099999998E-2</v>
+        <v>-9.12808539E-2</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>4.4563437099999999E-2</v>
+        <v>-1.223313541</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
-        <v>-1.9212081699999998E-2</v>
+        <v>-7.6031650499999994</v>
       </c>
       <c r="H3">
         <f t="shared" si="0"/>
-        <v>1.3517211499999999</v>
+        <v>1.2535056234999999</v>
       </c>
       <c r="I3">
         <f t="shared" si="0"/>
-        <v>-6.8778617600000008E-2</v>
+        <v>4.0615335119999996</v>
       </c>
       <c r="J3">
         <f t="shared" si="0"/>
-        <v>-5.2052172999999993E-2</v>
+        <v>-4.4711517556000002E-2</v>
       </c>
       <c r="K3">
         <f t="shared" si="0"/>
-        <v>0.1095685155</v>
+        <v>4.6344104599999998</v>
       </c>
       <c r="L3">
         <f t="shared" si="0"/>
-        <v>-1.007540904E-3</v>
+        <v>1.2890911222000001</v>
       </c>
       <c r="M3">
         <f t="shared" si="0"/>
-        <v>-4.3176432199999995E-3</v>
+        <v>-12.718149426</v>
       </c>
       <c r="N3">
         <f t="shared" si="0"/>
-        <v>14.8242432</v>
+        <v>-18.285397287999999</v>
       </c>
       <c r="O3">
         <f t="shared" si="0"/>
-        <v>0.34730653839999998</v>
+        <v>0.196382116</v>
       </c>
       <c r="P3">
         <f t="shared" si="0"/>
-        <v>-7.6117482299999997E-2</v>
+        <v>-3.4240472616999997</v>
       </c>
       <c r="Q3">
         <f t="shared" si="0"/>
-        <v>-0.36237136469999998</v>
+        <v>10.939013662999999</v>
       </c>
       <c r="R3">
         <f t="shared" si="0"/>
-        <v>-8.2203844800000005E-3</v>
+        <v>-4.6595941989999998</v>
       </c>
       <c r="S3">
         <f t="shared" si="0"/>
-        <v>1.259572863</v>
+        <v>1.5437468869000002</v>
       </c>
       <c r="T3">
         <f t="shared" si="0"/>
-        <v>-0.14633412400000001</v>
+        <v>-22.257962864</v>
       </c>
       <c r="U3">
         <f t="shared" si="0"/>
-        <v>-3.5136336599999998E-2</v>
+        <v>-0.54717066450000007</v>
       </c>
       <c r="V3">
         <f t="shared" si="0"/>
-        <v>-0.2097177318</v>
+        <v>2.1851635908000002</v>
       </c>
       <c r="W3">
         <f t="shared" si="0"/>
-        <v>-0.3709403127</v>
+        <v>1.2635066400000001</v>
       </c>
       <c r="X3">
         <f t="shared" si="0"/>
-        <v>8.9245969699999997E-2</v>
+        <v>1.9438716825000002</v>
       </c>
       <c r="Y3">
         <f t="shared" si="0"/>
-        <v>0.25006267320000003</v>
+        <v>-3.8551275578999997E-2</v>
       </c>
       <c r="Z3">
         <f t="shared" si="0"/>
-        <v>-0.21624014999999996</v>
+        <v>-2.1907234687999999</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4">
         <f>B1*B1</f>
-        <v>7.4578148100000005E-2</v>
+        <v>84.9661776441</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:Z4" si="1">C1*C1</f>
-        <v>0.37175847840000004</v>
+        <v>18.130478840100004</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>0.25981447839999994</v>
+        <v>19.582572048400003</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>2.4620748099999999E-2</v>
+        <v>0.15770032322499999</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>0.10517697609999999</v>
+        <v>8.3018896899999994</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
-        <v>2.8247524899999998E-2</v>
+        <v>23.784641302499999</v>
       </c>
       <c r="H4">
         <f t="shared" si="1"/>
-        <v>3.0102250000000002</v>
+        <v>62.568891002500003</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>6.8100121600000009E-4</v>
+        <v>59.423284822499994</v>
       </c>
       <c r="J4">
         <f t="shared" si="1"/>
-        <v>1.2611289999999999E-2</v>
+        <v>46.931542435600008</v>
       </c>
       <c r="K4">
         <f t="shared" si="1"/>
-        <v>3.6355048899999999E-2</v>
+        <v>20.371230902499999</v>
       </c>
       <c r="L4">
         <f t="shared" si="1"/>
-        <v>1.6388732889999998E-3</v>
+        <v>64.500494688399996</v>
       </c>
       <c r="M4">
         <f t="shared" si="1"/>
-        <v>7.7935888899999986E-2</v>
+        <v>29.105917100100001</v>
       </c>
       <c r="N4">
         <f t="shared" si="1"/>
-        <v>24.920064</v>
+        <v>49.248534352900002</v>
       </c>
       <c r="O4">
         <f t="shared" si="1"/>
-        <v>0.48488939559999994</v>
+        <v>34.562640999999992</v>
       </c>
       <c r="P4">
         <f t="shared" si="1"/>
-        <v>0.64152090250000005</v>
+        <v>34.549590852099996</v>
       </c>
       <c r="Q4">
         <f t="shared" si="1"/>
-        <v>0.14587052489999999</v>
+        <v>39.582846420099997</v>
       </c>
       <c r="R4">
         <f t="shared" si="1"/>
-        <v>0.2248466724</v>
+        <v>22.502689689999997</v>
       </c>
       <c r="S4">
         <f t="shared" si="1"/>
-        <v>2.1278056900000002</v>
+        <v>2.6504816809000005</v>
       </c>
       <c r="T4">
         <f t="shared" si="1"/>
-        <v>1.2018736900000002E-2</v>
+        <v>73.15141417960001</v>
       </c>
       <c r="U4">
         <f t="shared" si="1"/>
-        <v>0.56340036000000004</v>
+        <v>14.230171844099999</v>
       </c>
       <c r="V4">
         <f t="shared" si="1"/>
-        <v>0.32128491240000001</v>
+        <v>35.280273678400007</v>
       </c>
       <c r="W4">
         <f t="shared" si="1"/>
-        <v>0.41382202410000002</v>
+        <v>14.70875904</v>
       </c>
       <c r="X4">
         <f t="shared" si="1"/>
-        <v>3.3903856899999994E-2</v>
+        <v>40.157442260099998</v>
       </c>
       <c r="Y4">
         <f t="shared" si="1"/>
-        <v>0.38930112360000008</v>
+        <v>22.9691106121</v>
       </c>
       <c r="Z4">
         <f t="shared" si="1"/>
-        <v>8.2368999999999984E-2</v>
+        <v>28.076963512900001</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5">
         <f>B2*B2</f>
-        <v>0.38956322249999997</v>
+        <v>0.22121030890000001</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:Z5" si="2">C2*C2</f>
-        <v>0.39032505759999997</v>
+        <v>5.6135824899999999E-2</v>
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
-        <v>6.7790522250000011E-3</v>
+        <v>2.2359220900000003</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
-        <v>4.0405020099999994E-2</v>
+        <v>5.2835619600000001E-2</v>
       </c>
       <c r="F5">
         <f t="shared" si="2"/>
-        <v>1.88815081E-2</v>
+        <v>0.18025968489999999</v>
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>1.3066776099999998E-2</v>
+        <v>2.4304809999999999</v>
       </c>
       <c r="H5">
         <f t="shared" si="2"/>
-        <v>0.60698122809999988</v>
+        <v>2.51127409E-2</v>
       </c>
       <c r="I5">
         <f t="shared" si="2"/>
-        <v>6.946387360000001</v>
+        <v>0.27760253439999999</v>
       </c>
       <c r="J5">
         <f t="shared" si="2"/>
-        <v>0.21484152009999999</v>
+        <v>4.2596507559999994E-5</v>
       </c>
       <c r="K5">
         <f t="shared" si="2"/>
-        <v>0.33022262250000001</v>
+        <v>1.05431824</v>
       </c>
       <c r="L5">
         <f t="shared" si="2"/>
-        <v>6.1941254400000006E-4</v>
+        <v>2.5763460100000003E-2</v>
       </c>
       <c r="M5">
         <f t="shared" si="2"/>
-        <v>2.3919715600000002E-4</v>
+        <v>5.5573347600000007</v>
       </c>
       <c r="N5">
         <f t="shared" si="2"/>
-        <v>8.8185241599999991</v>
+        <v>6.78915136</v>
       </c>
       <c r="O5">
         <f t="shared" si="2"/>
-        <v>0.24876153759999997</v>
+        <v>1.1158272160000002E-3</v>
       </c>
       <c r="P5">
         <f t="shared" si="2"/>
-        <v>9.0314611559999987E-3</v>
+        <v>0.33934120089999997</v>
       </c>
       <c r="Q5">
         <f t="shared" si="2"/>
-        <v>0.90020246410000004</v>
+        <v>3.0230776899999996</v>
       </c>
       <c r="R5">
         <f t="shared" si="2"/>
-        <v>3.0053689600000001E-4</v>
+        <v>0.96485435289999999</v>
       </c>
       <c r="S5">
         <f t="shared" si="2"/>
-        <v>0.74561498009999994</v>
+        <v>0.89914013290000006</v>
       </c>
       <c r="T5">
         <f t="shared" si="2"/>
-        <v>1.7816910399999999</v>
+        <v>6.7724857599999995</v>
       </c>
       <c r="U5">
         <f t="shared" si="2"/>
-        <v>2.1912697209999998E-3</v>
+        <v>2.1039502500000005E-2</v>
       </c>
       <c r="V5">
         <f t="shared" si="2"/>
-        <v>0.13689260009999998</v>
+        <v>0.1353430521</v>
       </c>
       <c r="W5">
         <f t="shared" si="2"/>
-        <v>0.33250215689999996</v>
+        <v>0.10853730250000002</v>
       </c>
       <c r="X5">
         <f t="shared" si="2"/>
-        <v>0.23492439610000002</v>
+        <v>9.4095562500000007E-2</v>
       </c>
       <c r="Y5">
         <f t="shared" si="2"/>
-        <v>0.16062460840000001</v>
+        <v>6.470432720999999E-5</v>
       </c>
       <c r="Z5">
         <f t="shared" si="2"/>
-        <v>0.56768690249999998</v>
+        <v>0.17093263359999997</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="C8">
         <f>SUM(B3:Z3)</f>
-        <v>17.330724469895994</v>
+        <v>-55.735084694134983</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>0</v>
       </c>
       <c r="C9">
         <f>SQRT( SUM(B4:Z4))</f>
-        <v>5.8621447146590482</v>
+        <v>29.146110202274421</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10">
         <f>SQRT( SUM(B5:Z5))</f>
-        <v>4.7851081587147011</v>
+        <v>5.6067992599745162</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11">
         <f>C8/(C9*C10)</f>
-        <v>0.6178291908045852</v>
+        <v>-0.34106178086893379</v>
+      </c>
+      <c r="F11">
+        <v>-21.365194937110999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>4.7072399999999996</v>
+      </c>
+      <c r="B18">
+        <v>5.2690599999999996</v>
+      </c>
+      <c r="C18">
+        <v>1.2572300000000001</v>
+      </c>
+      <c r="D18">
+        <v>5.9212999999999996</v>
+      </c>
+      <c r="E18">
+        <v>4.5714899999999998</v>
+      </c>
+      <c r="F18">
+        <v>5.32742</v>
+      </c>
+      <c r="G18">
+        <v>3.3441100000000001</v>
+      </c>
+      <c r="H18">
+        <v>5.5971900000000003</v>
+      </c>
+      <c r="I18">
+        <v>7.1109299999999998</v>
+      </c>
+      <c r="J18">
+        <v>5.0204300000000002</v>
+      </c>
+      <c r="K18">
+        <v>7.3491400000000002</v>
+      </c>
+      <c r="L18">
+        <v>3.90632</v>
+      </c>
+      <c r="M18">
+        <v>2.9011100000000001</v>
+      </c>
+      <c r="N18">
+        <v>6.3213600000000003</v>
+      </c>
+      <c r="O18">
+        <v>3.7494499999999999</v>
+      </c>
+      <c r="P18">
+        <v>7.9719300000000004</v>
+      </c>
+      <c r="Q18">
+        <v>3.3418399999999999</v>
+      </c>
+      <c r="R18">
+        <v>-0.118245</v>
+      </c>
+      <c r="S18">
+        <v>3.2225899999999998</v>
+      </c>
+      <c r="T18">
+        <v>3.9204400000000001</v>
+      </c>
+      <c r="U18">
+        <v>7.0384500000000001</v>
+      </c>
+      <c r="V18">
+        <v>3.7420900000000001</v>
+      </c>
+      <c r="W18">
+        <v>4.0348199999999999</v>
+      </c>
+      <c r="X18">
+        <v>5.6791700000000001</v>
+      </c>
+      <c r="Y18">
+        <v>4.75739</v>
+      </c>
+      <c r="Z18">
+        <v>9.2177100000000003</v>
+      </c>
+      <c r="AA18">
+        <v>4.2579900000000004</v>
+      </c>
+      <c r="AB18">
+        <v>4.4252200000000004</v>
+      </c>
+      <c r="AC18">
+        <v>0.397115</v>
+      </c>
+      <c r="AD18">
+        <v>2.8813</v>
+      </c>
+      <c r="AE18">
+        <v>4.8769499999999999</v>
+      </c>
+      <c r="AF18">
+        <v>7.91005</v>
+      </c>
+      <c r="AG18">
+        <v>7.7086499999999996</v>
+      </c>
+      <c r="AH18">
+        <v>6.8506600000000004</v>
+      </c>
+      <c r="AI18">
+        <v>4.5134499999999997</v>
+      </c>
+      <c r="AJ18">
+        <v>8.0312199999999994</v>
+      </c>
+      <c r="AK18">
+        <v>5.39499</v>
+      </c>
+      <c r="AL18">
+        <v>7.0177300000000002</v>
+      </c>
+      <c r="AM18">
+        <v>5.8789999999999996</v>
+      </c>
+      <c r="AN18">
+        <v>5.8778899999999998</v>
+      </c>
+      <c r="AO18">
+        <v>6.2914899999999996</v>
+      </c>
+      <c r="AP18">
+        <v>4.7436999999999996</v>
+      </c>
+      <c r="AQ18">
+        <v>1.6280300000000001</v>
+      </c>
+      <c r="AR18">
+        <v>8.5528600000000008</v>
+      </c>
+      <c r="AS18">
+        <v>3.7722899999999999</v>
+      </c>
+      <c r="AT18">
+        <v>5.9397200000000003</v>
+      </c>
+      <c r="AU18">
+        <v>3.8351999999999999</v>
+      </c>
+      <c r="AV18">
+        <v>6.3369900000000001</v>
+      </c>
+      <c r="AW18">
+        <v>4.7926099999999998</v>
+      </c>
+      <c r="AX18">
+        <v>5.2987700000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>-0.47033000000000003</v>
+      </c>
+      <c r="B19">
+        <v>-0.23693</v>
+      </c>
+      <c r="C19">
+        <v>-1.4953000000000001</v>
+      </c>
+      <c r="D19">
+        <v>-0.22986000000000001</v>
+      </c>
+      <c r="E19">
+        <v>-0.42457</v>
+      </c>
+      <c r="F19">
+        <v>-1.5589999999999999</v>
+      </c>
+      <c r="G19">
+        <v>0.15847</v>
+      </c>
+      <c r="H19">
+        <v>0.52688000000000001</v>
+      </c>
+      <c r="I19">
+        <v>-6.5265999999999996E-3</v>
+      </c>
+      <c r="J19">
+        <v>1.0267999999999999</v>
+      </c>
+      <c r="K19">
+        <v>0.16051000000000001</v>
+      </c>
+      <c r="L19">
+        <v>-2.3574000000000002</v>
+      </c>
+      <c r="M19">
+        <v>-2.6055999999999999</v>
+      </c>
+      <c r="N19">
+        <v>3.3404000000000003E-2</v>
+      </c>
+      <c r="O19">
+        <v>-0.58252999999999999</v>
+      </c>
+      <c r="P19">
+        <v>1.7386999999999999</v>
+      </c>
+      <c r="Q19">
+        <v>-0.98226999999999998</v>
+      </c>
+      <c r="R19">
+        <v>0.94823000000000002</v>
+      </c>
+      <c r="S19">
+        <v>-2.6023999999999998</v>
+      </c>
+      <c r="T19">
+        <v>-0.14505000000000001</v>
+      </c>
+      <c r="U19">
+        <v>0.36788999999999999</v>
+      </c>
+      <c r="V19">
+        <v>0.32945000000000002</v>
+      </c>
+      <c r="W19">
+        <v>0.30675000000000002</v>
+      </c>
+      <c r="X19">
+        <v>-8.0438999999999997E-3</v>
+      </c>
+      <c r="Y19">
+        <v>-0.41343999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MemOpt is working. Refactored out code snippets. Starting on Simhash
</commit_message>
<xml_diff>
--- a/Untitled-1.xlsx
+++ b/Untitled-1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\petur\source\repos\ThesisParser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5CED27-5069-418F-8CAD-9E32109FD232}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B528F6C-EDC4-4203-9719-B45277E79FFA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -538,8 +538,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -895,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX19"/>
+  <dimension ref="A1:Z34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,79 +909,79 @@
         <v>4</v>
       </c>
       <c r="B1">
-        <v>9.2177100000000003</v>
+        <v>0.49653000000000003</v>
       </c>
       <c r="C1">
-        <v>4.2579900000000004</v>
+        <v>1.1435</v>
       </c>
       <c r="D1">
-        <v>4.4252200000000004</v>
+        <v>-0.28609000000000001</v>
       </c>
       <c r="E1">
-        <v>0.397115</v>
+        <v>-0.63378000000000001</v>
       </c>
       <c r="F1">
-        <v>2.8813</v>
+        <v>-1.2346999999999999</v>
       </c>
       <c r="G1">
-        <v>4.8769499999999999</v>
+        <v>-9.6415000000000001E-2</v>
       </c>
       <c r="H1">
-        <v>7.91005</v>
+        <v>0.81466000000000005</v>
       </c>
       <c r="I1">
-        <v>7.7086499999999996</v>
+        <v>0.31406000000000001</v>
       </c>
       <c r="J1">
-        <v>6.8506600000000004</v>
+        <v>-0.81064000000000003</v>
       </c>
       <c r="K1">
-        <v>4.5134499999999997</v>
+        <v>0.43028</v>
       </c>
       <c r="L1">
-        <v>8.0312199999999994</v>
+        <v>-0.10843999999999999</v>
       </c>
       <c r="M1">
-        <v>5.39499</v>
+        <v>0.23407</v>
       </c>
       <c r="N1">
-        <v>7.0177300000000002</v>
+        <v>-5.5358999999999998</v>
       </c>
       <c r="O1">
-        <v>5.8789999999999996</v>
+        <v>4.5616999999999998E-2</v>
       </c>
       <c r="P1">
-        <v>5.8778899999999998</v>
+        <v>-0.15731999999999999</v>
       </c>
       <c r="Q1">
-        <v>6.2914899999999996</v>
+        <v>0.74855000000000005</v>
       </c>
       <c r="R1">
-        <v>4.7436999999999996</v>
+        <v>0.35315000000000002</v>
       </c>
       <c r="S1">
-        <v>1.6280300000000001</v>
+        <v>-0.11169</v>
       </c>
       <c r="T1">
-        <v>8.5528600000000008</v>
+        <v>-0.12048</v>
       </c>
       <c r="U1">
-        <v>3.7722899999999999</v>
+        <v>-0.13965</v>
       </c>
       <c r="V1">
-        <v>5.9397200000000003</v>
+        <v>-0.27711000000000002</v>
       </c>
       <c r="W1">
-        <v>3.8351999999999999</v>
+        <v>0.34342</v>
       </c>
       <c r="X1">
-        <v>6.3369900000000001</v>
+        <v>-0.40377000000000002</v>
       </c>
       <c r="Y1">
-        <v>4.7926099999999998</v>
+        <v>0.61924000000000001</v>
       </c>
       <c r="Z1">
-        <v>5.2987700000000002</v>
+        <v>0.53939999999999999</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
@@ -988,79 +989,79 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>-0.47033000000000003</v>
+        <v>0.48304000000000002</v>
       </c>
       <c r="C2">
-        <v>-0.23693</v>
+        <v>1.4098999999999999</v>
       </c>
       <c r="D2">
-        <v>-1.4953000000000001</v>
+        <v>0.14266999999999999</v>
       </c>
       <c r="E2">
-        <v>-0.22986000000000001</v>
+        <v>1.1223000000000001</v>
       </c>
       <c r="F2">
-        <v>-0.42457</v>
+        <v>0.81710000000000005</v>
       </c>
       <c r="G2">
-        <v>-1.5589999999999999</v>
+        <v>1.7870999999999999</v>
       </c>
       <c r="H2">
-        <v>0.15847</v>
+        <v>-0.35749999999999998</v>
       </c>
       <c r="I2">
-        <v>0.52688000000000001</v>
+        <v>2.9927999999999999</v>
       </c>
       <c r="J2">
-        <v>-6.5265999999999996E-3</v>
+        <v>-0.55962000000000001</v>
       </c>
       <c r="K2">
-        <v>1.0267999999999999</v>
+        <v>-1.7713000000000001</v>
       </c>
       <c r="L2">
-        <v>0.16051000000000001</v>
+        <v>0.86858999999999997</v>
       </c>
       <c r="M2">
-        <v>-2.3574000000000002</v>
+        <v>-3.0158</v>
       </c>
       <c r="N2">
-        <v>-2.6055999999999999</v>
+        <v>-1.6781999999999999</v>
       </c>
       <c r="O2">
-        <v>3.3404000000000003E-2</v>
+        <v>-0.27716000000000002</v>
       </c>
       <c r="P2">
-        <v>-0.58252999999999999</v>
+        <v>1.8177000000000001</v>
       </c>
       <c r="Q2">
-        <v>1.7386999999999999</v>
+        <v>1.0758000000000001</v>
       </c>
       <c r="R2">
-        <v>-0.98226999999999998</v>
+        <v>-0.1075</v>
       </c>
       <c r="S2">
-        <v>0.94823000000000002</v>
+        <v>0.31785000000000002</v>
       </c>
       <c r="T2">
-        <v>-2.6023999999999998</v>
+        <v>0.40817999999999999</v>
       </c>
       <c r="U2">
-        <v>-0.14505000000000001</v>
+        <v>2.2583E-3</v>
       </c>
       <c r="V2">
-        <v>0.36788999999999999</v>
+        <v>-8.6491999999999999E-2</v>
       </c>
       <c r="W2">
-        <v>0.32945000000000002</v>
+        <v>-0.89681</v>
       </c>
       <c r="X2">
-        <v>0.30675000000000002</v>
+        <v>-0.11579</v>
       </c>
       <c r="Y2">
-        <v>-8.0438999999999997E-3</v>
+        <v>1.0685</v>
       </c>
       <c r="Z2">
-        <v>-0.41343999999999997</v>
+        <v>0.19672999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -1069,103 +1070,103 @@
       </c>
       <c r="B3">
         <f>B1*B2</f>
-        <v>-4.3353655443000001</v>
+        <v>0.23984385120000001</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:Z3" si="0">C1*C2</f>
-        <v>-1.0088455707000001</v>
+        <f>C1*C2</f>
+        <v>1.6122206499999998</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
-        <v>-6.6170314660000011</v>
+        <f>D1*D2</f>
+        <v>-4.0816460299999996E-2</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
-        <v>-9.12808539E-2</v>
+        <f>E1*E2</f>
+        <v>-0.71129129400000002</v>
       </c>
       <c r="F3">
-        <f t="shared" si="0"/>
-        <v>-1.223313541</v>
+        <f>F1*F2</f>
+        <v>-1.0088733699999999</v>
       </c>
       <c r="G3">
-        <f t="shared" si="0"/>
-        <v>-7.6031650499999994</v>
+        <f>G1*G2</f>
+        <v>-0.17230324649999998</v>
       </c>
       <c r="H3">
-        <f t="shared" si="0"/>
-        <v>1.2535056234999999</v>
+        <f>H1*H2</f>
+        <v>-0.29124095</v>
       </c>
       <c r="I3">
-        <f t="shared" si="0"/>
-        <v>4.0615335119999996</v>
+        <f>I1*I2</f>
+        <v>0.93991876799999996</v>
       </c>
       <c r="J3">
-        <f t="shared" si="0"/>
-        <v>-4.4711517556000002E-2</v>
+        <f>J1*J2</f>
+        <v>0.45365035680000004</v>
       </c>
       <c r="K3">
-        <f t="shared" si="0"/>
-        <v>4.6344104599999998</v>
+        <f>K1*K2</f>
+        <v>-0.76215496400000005</v>
       </c>
       <c r="L3">
-        <f t="shared" si="0"/>
-        <v>1.2890911222000001</v>
+        <f>L1*L2</f>
+        <v>-9.4189899599999988E-2</v>
       </c>
       <c r="M3">
-        <f t="shared" si="0"/>
-        <v>-12.718149426</v>
+        <f>M1*M2</f>
+        <v>-0.70590830599999999</v>
       </c>
       <c r="N3">
-        <f t="shared" si="0"/>
-        <v>-18.285397287999999</v>
+        <f>N1*N2</f>
+        <v>9.29034738</v>
       </c>
       <c r="O3">
-        <f t="shared" si="0"/>
-        <v>0.196382116</v>
+        <f>O1*O2</f>
+        <v>-1.2643207720000001E-2</v>
       </c>
       <c r="P3">
-        <f t="shared" si="0"/>
-        <v>-3.4240472616999997</v>
+        <f>P1*P2</f>
+        <v>-0.28596056399999997</v>
       </c>
       <c r="Q3">
-        <f t="shared" si="0"/>
-        <v>10.939013662999999</v>
+        <f>Q1*Q2</f>
+        <v>0.80529009000000007</v>
       </c>
       <c r="R3">
-        <f t="shared" si="0"/>
-        <v>-4.6595941989999998</v>
+        <f>R1*R2</f>
+        <v>-3.7963625000000001E-2</v>
       </c>
       <c r="S3">
-        <f t="shared" si="0"/>
-        <v>1.5437468869000002</v>
+        <f>S1*S2</f>
+        <v>-3.55006665E-2</v>
       </c>
       <c r="T3">
-        <f t="shared" si="0"/>
-        <v>-22.257962864</v>
+        <f>T1*T2</f>
+        <v>-4.9177526399999998E-2</v>
       </c>
       <c r="U3">
-        <f t="shared" si="0"/>
-        <v>-0.54717066450000007</v>
+        <f>U1*U2</f>
+        <v>-3.1537159500000001E-4</v>
       </c>
       <c r="V3">
-        <f t="shared" si="0"/>
-        <v>2.1851635908000002</v>
+        <f>V1*V2</f>
+        <v>2.3967798120000001E-2</v>
       </c>
       <c r="W3">
-        <f t="shared" si="0"/>
-        <v>1.2635066400000001</v>
+        <f>W1*W2</f>
+        <v>-0.30798249020000001</v>
       </c>
       <c r="X3">
-        <f t="shared" si="0"/>
-        <v>1.9438716825000002</v>
+        <f>X1*X2</f>
+        <v>4.6752528300000006E-2</v>
       </c>
       <c r="Y3">
-        <f t="shared" si="0"/>
-        <v>-3.8551275578999997E-2</v>
+        <f>Y1*Y2</f>
+        <v>0.66165794</v>
       </c>
       <c r="Z3">
-        <f t="shared" si="0"/>
-        <v>-2.1907234687999999</v>
+        <f>Z1*Z2</f>
+        <v>0.10611616199999999</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -1174,103 +1175,103 @@
       </c>
       <c r="B4">
         <f>B1*B1</f>
-        <v>84.9661776441</v>
+        <v>0.24654204090000004</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:Z4" si="1">C1*C1</f>
-        <v>18.130478840100004</v>
+        <f>C1*C1</f>
+        <v>1.3075922499999999</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
-        <v>19.582572048400003</v>
+        <f>D1*D1</f>
+        <v>8.1847488100000004E-2</v>
       </c>
       <c r="E4">
-        <f t="shared" si="1"/>
-        <v>0.15770032322499999</v>
+        <f>E1*E1</f>
+        <v>0.40167708839999999</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
-        <v>8.3018896899999994</v>
+        <f>F1*F1</f>
+        <v>1.5244840899999998</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
-        <v>23.784641302499999</v>
+        <f>G1*G1</f>
+        <v>9.2958522249999998E-3</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
-        <v>62.568891002500003</v>
+        <f>H1*H1</f>
+        <v>0.66367091560000013</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
-        <v>59.423284822499994</v>
+        <f>I1*I1</f>
+        <v>9.8633683600000008E-2</v>
       </c>
       <c r="J4">
-        <f t="shared" si="1"/>
-        <v>46.931542435600008</v>
+        <f>J1*J1</f>
+        <v>0.65713720959999999</v>
       </c>
       <c r="K4">
-        <f t="shared" si="1"/>
-        <v>20.371230902499999</v>
+        <f>K1*K1</f>
+        <v>0.18514087839999999</v>
       </c>
       <c r="L4">
-        <f t="shared" si="1"/>
-        <v>64.500494688399996</v>
+        <f>L1*L1</f>
+        <v>1.1759233599999998E-2</v>
       </c>
       <c r="M4">
-        <f t="shared" si="1"/>
-        <v>29.105917100100001</v>
+        <f>M1*M1</f>
+        <v>5.4788764900000002E-2</v>
       </c>
       <c r="N4">
-        <f t="shared" si="1"/>
-        <v>49.248534352900002</v>
+        <f>N1*N1</f>
+        <v>30.646188809999998</v>
       </c>
       <c r="O4">
-        <f t="shared" si="1"/>
-        <v>34.562640999999992</v>
+        <f>O1*O1</f>
+        <v>2.0809106889999999E-3</v>
       </c>
       <c r="P4">
-        <f t="shared" si="1"/>
-        <v>34.549590852099996</v>
+        <f>P1*P1</f>
+        <v>2.4749582399999998E-2</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="1"/>
-        <v>39.582846420099997</v>
+        <f>Q1*Q1</f>
+        <v>0.56032710250000006</v>
       </c>
       <c r="R4">
-        <f t="shared" si="1"/>
-        <v>22.502689689999997</v>
+        <f>R1*R1</f>
+        <v>0.12471492250000002</v>
       </c>
       <c r="S4">
-        <f t="shared" si="1"/>
-        <v>2.6504816809000005</v>
+        <f>S1*S1</f>
+        <v>1.24746561E-2</v>
       </c>
       <c r="T4">
-        <f t="shared" si="1"/>
-        <v>73.15141417960001</v>
+        <f>T1*T1</f>
+        <v>1.4515430400000001E-2</v>
       </c>
       <c r="U4">
-        <f t="shared" si="1"/>
-        <v>14.230171844099999</v>
+        <f>U1*U1</f>
+        <v>1.95021225E-2</v>
       </c>
       <c r="V4">
-        <f t="shared" si="1"/>
-        <v>35.280273678400007</v>
+        <f>V1*V1</f>
+        <v>7.6789952100000017E-2</v>
       </c>
       <c r="W4">
-        <f t="shared" si="1"/>
-        <v>14.70875904</v>
+        <f>W1*W1</f>
+        <v>0.1179372964</v>
       </c>
       <c r="X4">
-        <f t="shared" si="1"/>
-        <v>40.157442260099998</v>
+        <f>X1*X1</f>
+        <v>0.16303021290000003</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="1"/>
-        <v>22.9691106121</v>
+        <f>Y1*Y1</f>
+        <v>0.38345817760000001</v>
       </c>
       <c r="Z4">
-        <f t="shared" si="1"/>
-        <v>28.076963512900001</v>
+        <f>Z1*Z1</f>
+        <v>0.29095235999999997</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -1279,103 +1280,103 @@
       </c>
       <c r="B5">
         <f>B2*B2</f>
-        <v>0.22121030890000001</v>
+        <v>0.23332764160000002</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:Z5" si="2">C2*C2</f>
-        <v>5.6135824899999999E-2</v>
+        <f>C2*C2</f>
+        <v>1.9878180099999998</v>
       </c>
       <c r="D5">
-        <f t="shared" si="2"/>
-        <v>2.2359220900000003</v>
+        <f>D2*D2</f>
+        <v>2.0354728899999997E-2</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
-        <v>5.2835619600000001E-2</v>
+        <f>E2*E2</f>
+        <v>1.2595572900000003</v>
       </c>
       <c r="F5">
-        <f t="shared" si="2"/>
-        <v>0.18025968489999999</v>
+        <f>F2*F2</f>
+        <v>0.66765241000000008</v>
       </c>
       <c r="G5">
-        <f t="shared" si="2"/>
-        <v>2.4304809999999999</v>
+        <f>G2*G2</f>
+        <v>3.1937264099999996</v>
       </c>
       <c r="H5">
-        <f t="shared" si="2"/>
-        <v>2.51127409E-2</v>
+        <f>H2*H2</f>
+        <v>0.12780624999999998</v>
       </c>
       <c r="I5">
-        <f t="shared" si="2"/>
-        <v>0.27760253439999999</v>
+        <f>I2*I2</f>
+        <v>8.9568518399999988</v>
       </c>
       <c r="J5">
-        <f t="shared" si="2"/>
-        <v>4.2596507559999994E-5</v>
+        <f>J2*J2</f>
+        <v>0.31317454440000003</v>
       </c>
       <c r="K5">
-        <f t="shared" si="2"/>
-        <v>1.05431824</v>
+        <f>K2*K2</f>
+        <v>3.1375036900000004</v>
       </c>
       <c r="L5">
-        <f t="shared" si="2"/>
-        <v>2.5763460100000003E-2</v>
+        <f>L2*L2</f>
+        <v>0.75444858809999993</v>
       </c>
       <c r="M5">
-        <f t="shared" si="2"/>
-        <v>5.5573347600000007</v>
+        <f>M2*M2</f>
+        <v>9.0950496400000009</v>
       </c>
       <c r="N5">
-        <f t="shared" si="2"/>
-        <v>6.78915136</v>
+        <f>N2*N2</f>
+        <v>2.8163552399999996</v>
       </c>
       <c r="O5">
-        <f t="shared" si="2"/>
-        <v>1.1158272160000002E-3</v>
+        <f>O2*O2</f>
+        <v>7.6817665600000015E-2</v>
       </c>
       <c r="P5">
-        <f t="shared" si="2"/>
-        <v>0.33934120089999997</v>
+        <f>P2*P2</f>
+        <v>3.3040332900000005</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="2"/>
-        <v>3.0230776899999996</v>
+        <f>Q2*Q2</f>
+        <v>1.1573456400000002</v>
       </c>
       <c r="R5">
-        <f t="shared" si="2"/>
-        <v>0.96485435289999999</v>
+        <f>R2*R2</f>
+        <v>1.1556249999999999E-2</v>
       </c>
       <c r="S5">
-        <f t="shared" si="2"/>
-        <v>0.89914013290000006</v>
+        <f>S2*S2</f>
+        <v>0.10102862250000001</v>
       </c>
       <c r="T5">
-        <f t="shared" si="2"/>
-        <v>6.7724857599999995</v>
+        <f>T2*T2</f>
+        <v>0.16661091239999998</v>
       </c>
       <c r="U5">
-        <f t="shared" si="2"/>
-        <v>2.1039502500000005E-2</v>
+        <f>U2*U2</f>
+        <v>5.0999188899999998E-6</v>
       </c>
       <c r="V5">
-        <f t="shared" si="2"/>
-        <v>0.1353430521</v>
+        <f>V2*V2</f>
+        <v>7.4808660639999998E-3</v>
       </c>
       <c r="W5">
-        <f t="shared" si="2"/>
-        <v>0.10853730250000002</v>
+        <f>W2*W2</f>
+        <v>0.80426817610000001</v>
       </c>
       <c r="X5">
-        <f t="shared" si="2"/>
-        <v>9.4095562500000007E-2</v>
+        <f>X2*X2</f>
+        <v>1.3407324100000001E-2</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="2"/>
-        <v>6.470432720999999E-5</v>
+        <f>Y2*Y2</f>
+        <v>1.14169225</v>
       </c>
       <c r="Z5">
-        <f t="shared" si="2"/>
-        <v>0.17093263359999997</v>
+        <f>Z2*Z2</f>
+        <v>3.8702692899999995E-2</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -1384,7 +1385,7 @@
       </c>
       <c r="C8">
         <f>SUM(B3:Z3)</f>
-        <v>-55.735084694134983</v>
+        <v>9.663443582604998</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
@@ -1393,7 +1394,7 @@
       </c>
       <c r="C9">
         <f>SQRT( SUM(B4:Z4))</f>
-        <v>29.146110202274421</v>
+        <v>6.1383459524055821</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
@@ -1402,7 +1403,7 @@
       </c>
       <c r="C10">
         <f>SQRT( SUM(B5:Z5))</f>
-        <v>5.6067992599745162</v>
+        <v>6.2758724550920322</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
@@ -1411,240 +1412,195 @@
       </c>
       <c r="C11">
         <f>C8/(C9*C10)</f>
-        <v>-0.34106178086893379</v>
+        <v>0.25084557561041831</v>
       </c>
       <c r="F11">
         <v>-21.365194937110999</v>
       </c>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>4.7072399999999996</v>
-      </c>
-      <c r="B18">
-        <v>5.2690599999999996</v>
-      </c>
-      <c r="C18">
-        <v>1.2572300000000001</v>
-      </c>
-      <c r="D18">
-        <v>5.9212999999999996</v>
-      </c>
-      <c r="E18">
-        <v>4.5714899999999998</v>
-      </c>
-      <c r="F18">
-        <v>5.32742</v>
-      </c>
-      <c r="G18">
-        <v>3.3441100000000001</v>
-      </c>
-      <c r="H18">
-        <v>5.5971900000000003</v>
-      </c>
-      <c r="I18">
-        <v>7.1109299999999998</v>
-      </c>
-      <c r="J18">
-        <v>5.0204300000000002</v>
-      </c>
-      <c r="K18">
-        <v>7.3491400000000002</v>
-      </c>
-      <c r="L18">
-        <v>3.90632</v>
-      </c>
-      <c r="M18">
-        <v>2.9011100000000001</v>
-      </c>
-      <c r="N18">
-        <v>6.3213600000000003</v>
-      </c>
-      <c r="O18">
-        <v>3.7494499999999999</v>
-      </c>
-      <c r="P18">
-        <v>7.9719300000000004</v>
-      </c>
-      <c r="Q18">
-        <v>3.3418399999999999</v>
-      </c>
-      <c r="R18">
-        <v>-0.118245</v>
-      </c>
-      <c r="S18">
-        <v>3.2225899999999998</v>
-      </c>
-      <c r="T18">
-        <v>3.9204400000000001</v>
-      </c>
-      <c r="U18">
-        <v>7.0384500000000001</v>
-      </c>
-      <c r="V18">
-        <v>3.7420900000000001</v>
-      </c>
-      <c r="W18">
-        <v>4.0348199999999999</v>
-      </c>
-      <c r="X18">
-        <v>5.6791700000000001</v>
-      </c>
-      <c r="Y18">
-        <v>4.75739</v>
-      </c>
-      <c r="Z18">
-        <v>9.2177100000000003</v>
-      </c>
-      <c r="AA18">
-        <v>4.2579900000000004</v>
-      </c>
-      <c r="AB18">
-        <v>4.4252200000000004</v>
-      </c>
-      <c r="AC18">
-        <v>0.397115</v>
-      </c>
-      <c r="AD18">
-        <v>2.8813</v>
-      </c>
-      <c r="AE18">
-        <v>4.8769499999999999</v>
-      </c>
-      <c r="AF18">
-        <v>7.91005</v>
-      </c>
-      <c r="AG18">
-        <v>7.7086499999999996</v>
-      </c>
-      <c r="AH18">
-        <v>6.8506600000000004</v>
-      </c>
-      <c r="AI18">
-        <v>4.5134499999999997</v>
-      </c>
-      <c r="AJ18">
-        <v>8.0312199999999994</v>
-      </c>
-      <c r="AK18">
-        <v>5.39499</v>
-      </c>
-      <c r="AL18">
-        <v>7.0177300000000002</v>
-      </c>
-      <c r="AM18">
-        <v>5.8789999999999996</v>
-      </c>
-      <c r="AN18">
-        <v>5.8778899999999998</v>
-      </c>
-      <c r="AO18">
-        <v>6.2914899999999996</v>
-      </c>
-      <c r="AP18">
-        <v>4.7436999999999996</v>
-      </c>
-      <c r="AQ18">
-        <v>1.6280300000000001</v>
-      </c>
-      <c r="AR18">
-        <v>8.5528600000000008</v>
-      </c>
-      <c r="AS18">
-        <v>3.7722899999999999</v>
-      </c>
-      <c r="AT18">
-        <v>5.9397200000000003</v>
-      </c>
-      <c r="AU18">
-        <v>3.8351999999999999</v>
-      </c>
-      <c r="AV18">
-        <v>6.3369900000000001</v>
-      </c>
-      <c r="AW18">
-        <v>4.7926099999999998</v>
-      </c>
-      <c r="AX18">
-        <v>5.2987700000000002</v>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.11096</v>
+      </c>
+      <c r="B19">
+        <v>0.68901999999999997</v>
+      </c>
+      <c r="C19">
+        <v>5.3404E-2</v>
+      </c>
+      <c r="D19">
+        <v>0.88277000000000005</v>
+      </c>
+      <c r="E19">
+        <v>0.10493</v>
+      </c>
+      <c r="F19">
+        <v>0.96257000000000004</v>
+      </c>
+      <c r="G19">
+        <v>-0.15004000000000001</v>
+      </c>
+      <c r="H19">
+        <v>2.9756999999999998</v>
+      </c>
+      <c r="I19">
+        <v>-1.1916</v>
+      </c>
+      <c r="J19">
+        <v>-0.89127999999999996</v>
+      </c>
+      <c r="K19">
+        <v>0.64354999999999996</v>
+      </c>
+      <c r="L19">
+        <v>-2.7534999999999998</v>
+      </c>
+      <c r="M19">
+        <v>-1.5121</v>
+      </c>
+      <c r="N19">
+        <v>-0.69791000000000003</v>
+      </c>
+      <c r="O19">
+        <v>1.2213000000000001</v>
+      </c>
+      <c r="P19">
+        <v>1.1894</v>
+      </c>
+      <c r="Q19">
+        <v>4.9919999999999999E-2</v>
+      </c>
+      <c r="R19">
+        <v>1.0419</v>
+      </c>
+      <c r="S19">
+        <v>0.87226999999999999</v>
+      </c>
+      <c r="T19">
+        <v>-0.55386000000000002</v>
+      </c>
+      <c r="U19">
+        <v>0.34610999999999997</v>
+      </c>
+      <c r="V19">
+        <v>-0.81037000000000003</v>
+      </c>
+      <c r="W19">
+        <v>0.61826999999999999</v>
+      </c>
+      <c r="X19">
+        <v>2.2648999999999999</v>
+      </c>
+      <c r="Y19">
+        <v>0.45045000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>-0.47033000000000003</v>
-      </c>
-      <c r="B19">
-        <v>-0.23693</v>
-      </c>
-      <c r="C19">
-        <v>-1.4953000000000001</v>
-      </c>
-      <c r="D19">
-        <v>-0.22986000000000001</v>
-      </c>
-      <c r="E19">
-        <v>-0.42457</v>
-      </c>
-      <c r="F19">
-        <v>-1.5589999999999999</v>
-      </c>
-      <c r="G19">
-        <v>0.15847</v>
-      </c>
-      <c r="H19">
-        <v>0.52688000000000001</v>
-      </c>
-      <c r="I19">
-        <v>-6.5265999999999996E-3</v>
-      </c>
-      <c r="J19">
-        <v>1.0267999999999999</v>
-      </c>
-      <c r="K19">
-        <v>0.16051000000000001</v>
-      </c>
-      <c r="L19">
-        <v>-2.3574000000000002</v>
-      </c>
-      <c r="M19">
-        <v>-2.6055999999999999</v>
-      </c>
-      <c r="N19">
-        <v>3.3404000000000003E-2</v>
-      </c>
-      <c r="O19">
-        <v>-0.58252999999999999</v>
-      </c>
-      <c r="P19">
-        <v>1.7386999999999999</v>
-      </c>
-      <c r="Q19">
-        <v>-0.98226999999999998</v>
-      </c>
-      <c r="R19">
-        <v>0.94823000000000002</v>
-      </c>
-      <c r="S19">
-        <v>-2.6023999999999998</v>
-      </c>
-      <c r="T19">
-        <v>-0.14505000000000001</v>
-      </c>
-      <c r="U19">
-        <v>0.36788999999999999</v>
-      </c>
-      <c r="V19">
-        <v>0.32945000000000002</v>
-      </c>
-      <c r="W19">
-        <v>0.30675000000000002</v>
-      </c>
-      <c r="X19">
-        <v>-8.0438999999999997E-3</v>
-      </c>
-      <c r="Y19">
-        <v>-0.41343999999999997</v>
-      </c>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.49653000000000003</v>
+      </c>
+      <c r="B22">
+        <v>1.1435</v>
+      </c>
+      <c r="C22">
+        <v>-0.28609000000000001</v>
+      </c>
+      <c r="D22">
+        <v>-0.63378000000000001</v>
+      </c>
+      <c r="E22">
+        <v>-1.2346999999999999</v>
+      </c>
+      <c r="F22">
+        <v>-9.6415000000000001E-2</v>
+      </c>
+      <c r="G22">
+        <v>0.81466000000000005</v>
+      </c>
+      <c r="H22">
+        <v>0.31406000000000001</v>
+      </c>
+      <c r="I22">
+        <v>-0.81064000000000003</v>
+      </c>
+      <c r="J22">
+        <v>0.43028</v>
+      </c>
+      <c r="K22">
+        <v>-0.10843999999999999</v>
+      </c>
+      <c r="L22">
+        <v>0.23407</v>
+      </c>
+      <c r="M22">
+        <v>-5.5358999999999998</v>
+      </c>
+      <c r="N22">
+        <v>4.5616999999999998E-2</v>
+      </c>
+      <c r="O22">
+        <v>-0.15731999999999999</v>
+      </c>
+      <c r="P22">
+        <v>0.74855000000000005</v>
+      </c>
+      <c r="Q22">
+        <v>0.35315000000000002</v>
+      </c>
+      <c r="R22">
+        <v>-0.11169</v>
+      </c>
+      <c r="S22">
+        <v>-0.12048</v>
+      </c>
+      <c r="T22">
+        <v>-0.13965</v>
+      </c>
+      <c r="U22">
+        <v>-0.27711000000000002</v>
+      </c>
+      <c r="V22">
+        <v>0.34342</v>
+      </c>
+      <c r="W22">
+        <v>-0.40377000000000002</v>
+      </c>
+      <c r="X22">
+        <v>0.61924000000000001</v>
+      </c>
+      <c r="Y22">
+        <v>0.53939999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="X23" s="1"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="X30" s="1"/>
+    </row>
+    <row r="34" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="X34" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>